<commit_message>
adding even simpler tb
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb_simple.xlsx
+++ b/tests/databooks/databook_tb_simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{73AE4470-F459-8D4D-83B4-E8D4D9270C53}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{284159E1-2382-8945-864B-DDEB6545FD8F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{908129C3-6159-0448-B018-90A768D61B99}">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{47ED9844-02A3-184A-9FE8-DDC6DBFC62B9}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>Pren Naidoo, Grant Theron, Molebogeng X Rangaka, Violet N Chihota, Louise Vaughan, Zameer O Brey, Yogan Pillay; The South African Tuberculosis Care Cascade: Estimated Losses and Methodological Challenges, </t>
         </r>
@@ -66,7 +65,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The Journal of Infectious Diseases</t>
         </r>
@@ -76,7 +74,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>, Volume 216, Issue suppl_7, 6 November 2017, Pages S702–S713</t>
         </r>
@@ -131,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{7A69379A-5B1B-2C49-A4FE-556C850AB0CC}">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{1B592CC3-6877-9043-9BED-9D3CAA548799}">
       <text>
         <r>
           <rPr>
@@ -232,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{4D6C8F24-5DE6-6947-BE05-1A0A148F5DD9}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{2BB79B26-5B62-034E-A59D-D935DDC38F9B}">
       <text>
         <r>
           <rPr>
@@ -336,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{2E3F5F4F-18E2-AD4D-B78B-8E5BF34B3180}">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{1BE83851-7F38-484A-B347-14FDAA44B6A6}">
       <text>
         <r>
           <rPr>
@@ -440,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{50C072C8-8DE2-A849-A2B4-79B8AAF5A91D}">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{2524C9E8-EEB9-2A48-BB5F-79A1E57047F7}">
       <text>
         <r>
           <rPr>
@@ -541,54 +538,6 @@
             <family val="2"/>
           </rPr>
           <t>See: https://doi.org/10.1093/infdis/jix335</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{AD978786-588E-C247-864F-D1E30D67DF7C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Placeholder value</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{C66F225B-123A-674D-9996-FC1550184176}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Placeholder value</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
         </r>
       </text>
     </comment>
@@ -597,7 +546,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -605,7 +554,7 @@
     <t>Full Name</t>
   </si>
   <si>
-    <t>Population size</t>
+    <t>TB burden</t>
   </si>
   <si>
     <t>Units</t>
@@ -620,9 +569,6 @@
     <t>OR</t>
   </si>
   <si>
-    <t>TB burden</t>
-  </si>
-  <si>
     <t>Notified</t>
   </si>
   <si>
@@ -635,27 +581,21 @@
     <t>Successfully treated</t>
   </si>
   <si>
-    <t>Annual number of births</t>
-  </si>
-  <si>
-    <t>Estimated number of new TB cases annually</t>
-  </si>
-  <si>
-    <t>Annual number vaccinated</t>
-  </si>
-  <si>
     <t>Annual number of tests done</t>
   </si>
   <si>
+    <t>Test yield</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
     <t>Annual number newly initiated onto treatment</t>
   </si>
   <si>
     <t>Loss-to-follow-up rate</t>
   </si>
   <si>
-    <t>Probability</t>
-  </si>
-  <si>
     <t>Time after initiating treatment to treatment success (years)</t>
   </si>
   <si>
@@ -665,25 +605,10 @@
     <t>Treatment failure rate</t>
   </si>
   <si>
-    <t>Death rate for those with untreated TB</t>
-  </si>
-  <si>
-    <t>Death rate for those unsuccessfully treated</t>
-  </si>
-  <si>
-    <t>Death rate for those successfully treated</t>
-  </si>
-  <si>
-    <t>Background mortality rate</t>
-  </si>
-  <si>
     <t>adults</t>
   </si>
   <si>
     <t>Adults</t>
-  </si>
-  <si>
-    <t>Natural recovery rate</t>
   </si>
 </sst>
 </file>
@@ -707,16 +632,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -733,19 +671,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -826,103 +751,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -1413,10 +1242,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1429,20 +1258,18 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="3.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1484,15 +1311,10 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2">
-        <f>ROUND(F2*F2/G2,0)</f>
-        <v>53106065</v>
-      </c>
-      <c r="F2" s="2">
-        <v>54490000</v>
-      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="2">
-        <v>55910000</v>
+        <v>532005</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1539,7 +1361,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <v>532005</v>
+        <v>504514</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1586,7 +1408,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <v>504514</v>
+        <v>435483</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1633,7 +1455,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <v>435483</v>
+        <v>372577</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1680,127 +1502,71 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
-        <v>372577</v>
+        <v>279816</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G16" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H16" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I16" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>279816</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="37" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>AND(COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="35" priority="9">
+    <cfRule type="expression" dxfId="19" priority="9">
       <formula>COUNTIF(E14:I14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="10">
+    <cfRule type="expression" dxfId="18" priority="10">
       <formula>AND(COUNTIF(E14:I14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="33" priority="11">
-      <formula>COUNTIF(E17:I17,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="12">
-      <formula>AND(COUNTIF(E17:I17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="31" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>COUNTIF(E2:I2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>AND(COUNTIF(E2:I2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="29" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>COUNTIF(E5:I5,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>AND(COUNTIF(E5:I5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="27" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>COUNTIF(E8:I8,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>AND(COUNTIF(E8:I8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B17 B14 B11 B8 B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B14 B11 B8 B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1813,7 +1579,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1853,14 +1619,14 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
-        <v>564691</v>
+        <v>340632</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1891,7 +1657,7 @@
         <v>adults</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
@@ -1900,14 +1666,14 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <v>45900</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1938,23 +1704,23 @@
         <v>adults</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>15000</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -1985,7 +1751,7 @@
         <v>adults</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
@@ -1994,15 +1760,14 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <f>ROUND(G2*0.9,0)</f>
-        <v>508222</v>
+        <v>0.2</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -2033,24 +1798,23 @@
         <v>adults</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.2</v>
+      </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <f>ROUND(289537/0.85,0)</f>
-        <v>340632</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -2081,466 +1845,80 @@
         <v>adults</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.16</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>15000</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G19" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H19" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I19" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G22" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H22" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I22" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G25" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H25" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I25" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="4">
-        <v>0.16</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F28" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G28" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H28" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I28" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="4">
-        <v>0.12</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G31" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H31" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I31" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F34" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G34" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H34" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I34" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F37" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G37" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H37" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I37" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="11" priority="7">
+      <formula>COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="8">
+      <formula>AND(COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="25" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>COUNTIF(E14:I14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>AND(COUNTIF(E14:I14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="23" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>COUNTIF(E17:I17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="12">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>AND(COUNTIF(E17:I17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="21" priority="13">
-      <formula>COUNTIF(E20:I20,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14">
-      <formula>AND(COUNTIF(E20:I20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>COUNTIF(E2:I2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND(COUNTIF(E2:I2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="17" priority="15">
-      <formula>COUNTIF(E23:I23,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="16">
-      <formula>AND(COUNTIF(E23:I23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="15" priority="17">
-      <formula>COUNTIF(E26:I26,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="18">
-      <formula>AND(COUNTIF(E26:I26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="13" priority="19">
-      <formula>COUNTIF(E29:I29,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="20">
-      <formula>AND(COUNTIF(E29:I29,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="11" priority="21">
-      <formula>COUNTIF(E32:I32,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="22">
-      <formula>AND(COUNTIF(E32:I32,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="9" priority="23">
-      <formula>COUNTIF(E35:I35,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="24">
-      <formula>AND(COUNTIF(E35:I35,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="7" priority="25">
-      <formula>COUNTIF(E38:I38,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="26">
-      <formula>AND(COUNTIF(E38:I38,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>COUNTIF(E5:I5,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(COUNTIF(E5:I5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
-      <formula>AND(COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>COUNTIF(E8:I8,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>AND(COUNTIF(E8:I8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B17 B14 B11 B5" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B8" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20 B38 B35 B32 B29 B26 B8" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 B17 B11" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Probability"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23" xr:uid="{00000000-0002-0000-0200-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"Duration"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update simple tb example
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb_simple.xlsx
+++ b/tests/databooks/databook_tb_simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{284159E1-2382-8945-864B-DDEB6545FD8F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8E8A0A23-F2D3-1747-B413-13660BCE02D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="18300" windowHeight="15220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -546,7 +546,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -600,9 +600,6 @@
   </si>
   <si>
     <t>Duration</t>
-  </si>
-  <si>
-    <t>Treatment failure rate</t>
   </si>
   <si>
     <t>adults</t>
@@ -751,19 +748,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -1242,10 +1227,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1509,42 +1494,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="21" priority="7">
+    <cfRule type="expression" dxfId="19" priority="7">
       <formula>COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="18" priority="8">
       <formula>AND(COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="17" priority="9">
       <formula>COUNTIF(E14:I14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>AND(COUNTIF(E14:I14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>COUNTIF(E2:I2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>AND(COUNTIF(E2:I2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>COUNTIF(E5:I5,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>AND(COUNTIF(E5:I5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>COUNTIF(E8:I8,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>AND(COUNTIF(E8:I8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1563,10 +1548,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G11"/>
+      <selection activeCell="A16" sqref="A16:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1812,76 +1797,21 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G16" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H16" s="1">
-        <v>2017</v>
-      </c>
-      <c r="I16" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>adults</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.16</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>AND(COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>COUNTIF(E14:I14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>AND(COUNTIF(E14:I14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="7" priority="11">
-      <formula>COUNTIF(E17:I17,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12">
-      <formula>AND(COUNTIF(E17:I17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
@@ -1912,7 +1842,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B8" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 B17 B11" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 B11" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{00000000-0002-0000-0200-000004000000}">

</xml_diff>